<commit_message>
Update code to merge experimental data Data is connected to computational features by position and name ID.
</commit_message>
<xml_diff>
--- a/data/INSRTR_constructs.xlsx
+++ b/data/INSRTR_constructs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="217">
   <si>
     <t>Name</t>
   </si>
@@ -58,7 +58,7 @@
     <t>insert_index1</t>
   </si>
   <si>
-    <t>Active_site_residues</t>
+    <t>insert_index_manual_fix_1</t>
   </si>
   <si>
     <t>Lck_N266_P7</t>
@@ -88,6 +88,12 @@
     <t>Y</t>
   </si>
   <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>3,8</t>
+  </si>
+  <si>
     <t>not tested</t>
   </si>
   <si>
@@ -103,6 +109,9 @@
     <t>MGCGCSSHPEDDWMENIDVCENCHYPIVPLDGKGTLLIRNGSEVRDPLVTYEGSNPPASPLQDNLVIALHSYEPSHDGDLGFEKGEQLRILEQSGEWWKAQSLTTGQEGFIPFNFVAKANSLEPEPWFFKNLSRKDAERQLLAPGNTHGSFLIRESESTAGSFSLSVRDFDQNQGEVVKHYKIRNLDNGGFYISPRITFPGLHELVRHYTNASDGLCTRLSRPCQTQKPQKPWWEDEWEVPRETLKLVERLGAGQFGEVWMGYYNGHTKVAVKSLKQGGSSGSEIQALEEKNAQLKQEIAALEEKNQALKYGGSGGSSMSPDAFLAEANLMKQLQHQRLVRLYAVVTQEPIYIITEYMENGSLVDFLKTPSGIKLTINKLLDMAAQIAEGMAFIEERNYIHRDLRAANILVSDTLSCKIADFGLARLIEDNEYTAREGAKFPIKWTAPEAINYGTFTIKSDVWSFGILLTEIVTHGRIPYPGMTNPEVIQNLERGYRMVRPDNCPEELYQLMRLCWKERPEDRPTFDYLRSVLEDFFTATEGQYQPQP</t>
   </si>
   <si>
+    <t>1,7</t>
+  </si>
+  <si>
     <t>Lck_T375_P7</t>
   </si>
   <si>
@@ -115,6 +124,9 @@
     <t>GGSGGG</t>
   </si>
   <si>
+    <t>1,9</t>
+  </si>
+  <si>
     <t>Lck_Q256_P7</t>
   </si>
   <si>
@@ -169,42 +181,63 @@
     <t>MGESLFKGPRDYNPISSTICHLTNESDGGSSGSEIQALEEKNAQLKQEIAALEEKNQALKYGGSGGSHTTSLYGIGFGPFIITNKHLFRRNNGTLLVQSLHGVFKVKNTTTLQQHLIDGRDMIIIRMPKDFPPFPQKLKFREPQREERICLVTTNFQTKSMSSMVSDTSCTFPSSDGIFWKHWIQTKDGQCGSPLVSTRDGFIVGIHSASNFTNTNNYFTSVPKNFMELLTNQEAQQWVSGWRLNADSVLWGGHKVFMSKPEEPFQPVKEATQLMNEGGGLE</t>
   </si>
   <si>
+    <t>5,1</t>
+  </si>
+  <si>
     <t>TEVp_L72_P7</t>
   </si>
   <si>
     <t>MGESLFKGPRDYNPISSTICHLTNESDGHTTSLYGIGFGPFIITNKHLFRRNNGTLLVQSLHGVFKVKNTTTLGSSGSEIQALEEKNAQLKQEIAALEEKNQALKYGGSGGSQQHLIDGRDMIIIRMPKDFPPFPQKLKFREPQREERICLVTTNFQTKSMSSMVSDTSCTFPSSDGIFWKHWIQTKDGQCGSPLVSTRDGFIVGIHSASNFTNTNNYFTSVPKNFMELLTNQEAQQWVSGWRLNADSVLWGGHKVFMSKPEEPFQPVKEATQLMNEGGGLE</t>
   </si>
   <si>
+    <t>1,5</t>
+  </si>
+  <si>
     <t>TEVp_I77_P7</t>
   </si>
   <si>
     <t>MGESLFKGPRDYNPISSTICHLTNESDGHTTSLYGIGFGPFIITNKHLFRRNNGTLLVQSLHGVFKVKNTTTLQQHLIGSSGSEIQALEEKNAQLKQEIAALEEKNQALKYGGSGGSDGRDMIIIRMPKDFPPFPQKLKFREPQREERICLVTTNFQTKSMSSMVSDTSCTFPSSDGIFWKHWIQTKDGQCGSPLVSTRDGFIVGIHSASNFTNTNNYFTSVPKNFMELLTNQEAQQWVSGWRLNADSVLWGGHKVFMSKPEEPFQPVKEATQLMNEGGGLE</t>
   </si>
   <si>
+    <t>5,2</t>
+  </si>
+  <si>
     <t>TEVp_G79_P7</t>
   </si>
   <si>
     <t>MGESLFKGPRDYNPISSTICHLTNESDGHTTSLYGIGFGPFIITNKHLFRRNNGTLLVQSLHGVFKVKNTTTLQQHLIDGGSSGSEIQALEEKNAQLKQEIAALEEKNQALKYGGSGGSRDMIIIRMPKDFPPFPQKLKFREPQREERICLVTTNFQTKSMSSMVSDTSCTFPSSDGIFWKHWIQTKDGQCGSPLVSTRDGFIVGIHSASNFTNTNNYFTSVPKNFMELLTNQEAQQWVSGWRLNADSVLWGGHKVFMSKPEEPFQPVKEATQLMNEGGGLE</t>
   </si>
   <si>
+    <t>6,4</t>
+  </si>
+  <si>
     <t>TEVp_K147_P7</t>
   </si>
   <si>
     <t>MGESLFKGPRDYNPISSTICHLTNESDGHTTSLYGIGFGPFIITNKHLFRRNNGTLLVQSLHGVFKVKNTTTLQQHLIDGRDMIIIRMPKDFPPFPQKLKFREPQREERICLVTTNFQTKSMSSMVSDTSCTFPSSDGIFWKHWIQTKGSSGSEIQALEEKNAQLKQEIAALEEKNQALKYGGSGGSDGQCGSPLVSTRDGFIVGIHSASNFTNTNNYFTSVPKNFMELLTNQEAQQWVSGWRLNADSVLWGGHKVFMSKPEEPFQPVKEATQLMNEGGGLE</t>
   </si>
   <si>
+    <t>1,1</t>
+  </si>
+  <si>
     <t>TEVp_F172_P7</t>
   </si>
   <si>
     <t>MGESLFKGPRDYNPISSTICHLTNESDGHTTSLYGIGFGPFIITNKHLFRRNNGTLLVQSLHGVFKVKNTTTLQQHLIDGRDMIIIRMPKDFPPFPQKLKFREPQREERICLVTTNFQTKSMSSMVSDTSCTFPSSDGIFWKHWIQTKDGQCGSPLVSTRDGFIVGIHSASNFGSSGSEIQALEEKNAQLKQEIAALEEKNQALKYGGSGGSTNTNNYFTSVPKNFMELLTNQEAQQWVSGWRLNADSVLWGGHKVFMSKPEEPFQPVKEATQLMNEGGGLE</t>
   </si>
   <si>
+    <t>1,3</t>
+  </si>
+  <si>
     <t>TEVp_T175_P7</t>
   </si>
   <si>
     <t>MGESLFKGPRDYNPISSTICHLTNESDGHTTSLYGIGFGPFIITNKHLFRRNNGTLLVQSLHGVFKVKNTTTLQQHLIDGRDMIIIRMPKDFPPFPQKLKFREPQREERICLVTTNFQTKSMSSMVSDTSCTFPSSDGIFWKHWIQTKDGQCGSPLVSTRDGFIVGIHSASNFTNTGSSGSEIQALEEKNAQLKQEIAALEEKNQALKYGGSGGSNNYFTSVPKNFMELLTNQEAQQWVSGWRLNADSVLWGGHKVFMSKPEEPFQPVKEATQLMNEGGGLE</t>
   </si>
   <si>
+    <t>2,1</t>
+  </si>
+  <si>
     <t>TEVp_K184_P7</t>
   </si>
   <si>
@@ -217,6 +250,9 @@
     <t>MGESLFKGPRDYNPISSTICHLTNESDGHTTSLYGIGFGPFIITNKHLFRRNNGTLLVQSLHGVFKVKNTTTLQQHLIDGRDMIIIRMPKDFPPFPQKLKFREPQREERICLVTTNFQTKSMSSMVSDTSCTFPSSDGIFWKHWIQTKDGQCGSPLVSTRDGFIVGIHSASNFTNTNNYFTSVPKNFMELLTNQEAQQWVSGWRLNADSVLWGGSSGSEIQALEEKNAQLKQEIAALEEKNQALKYGGSGGSGHKVFMSKPEEPFQPVKEATQLMNEGGGLE</t>
   </si>
   <si>
+    <t>1,4</t>
+  </si>
+  <si>
     <t>TEVp_I77_AI</t>
   </si>
   <si>
@@ -229,6 +265,9 @@
     <t>ON</t>
   </si>
   <si>
+    <t>9,9</t>
+  </si>
+  <si>
     <t>N7</t>
   </si>
   <si>
@@ -241,6 +280,9 @@
     <t>MGESLFKGPRDYNPISSTICHLTNESDGGSSGSEIQALEEKNAQLKQEIAALEEKNQALKYGGSGGSHTTSLYGIGFGPFIITNKHLFRRNNGTLLVQSLHGVFKVKNTTTLQQHLIDGRDMIIIRMPKDFPPFPQKLKFREPQREERICLVTTNFQTKSMSSMVSDTSCTFPSSDGIFWKHWIQTKDGQCGSPLVSTRDGFIVGIHSASNFTNTNNYFTSVPKNFMELLTNQEAQQWVSGWRLNADSVLWGGHKVFMSKPEEPFQPVKEATQLMNEGGGLEGSPGGSPGGSGSPGGSPGGSKIAALKAENAALEAKIAALKAEIAALEAGY</t>
   </si>
   <si>
+    <t>7,2</t>
+  </si>
+  <si>
     <t>TEVp_G79_AI</t>
   </si>
   <si>
@@ -328,13 +370,13 @@
     <t>dCas_G1104</t>
   </si>
   <si>
-    <t>DKKYSIGLAIGTNSVGWAVITDEYKVPSKKFKVLGNTDRHSIKKNLIGALLFDSGETAEATRLKRTARRRYTRRKNRICYLQEIFSNEMAKVDDSFFHRLEESFLVEEDKKHERHPIFGNIVDEVAYHEKYPTIYHLRKKLVDSTDKADLRLIYLALAHMIKFRGHFLIEGDLNPDNSDVDKLFIQLVQTYNQLFEENPINASGVDAKAILSARLSKSRRLENLIAQLPGEKKNGLFGNLIALSLGLTPNFKSNFDLAEDAKLQLSKDTYDDDLDNLLAQIGDQYADLFLAAKNLSDAILLSDILRVNTEITKAPLSASMIKRYDEHHQDLTLLKALVRQQLPEKYKEIFFDQSKNGYAGYIDGGASQEEFYKFIKPILEKMDGTEELLVKLNREDLLRKQRTFDNGSIPHQIHLGELHAILRRQEDFYPFLKDNREKIEKILTFRIPYYVGPLARGNSRFAWMTRKSEETITPWNFEEVVDKGASAQSFIERMTNFDKNLPNEKVLPKHSLLYEYFTVYNELTKVKYVTEGMRKPAFLSGEQKKAIVDLLFKTNRKVTVKQLKEDYFKKIECFDSVEISGVEDRFNASLGTYHDLLKIIKDKDFLDNEENEDILEDIVLTLTLFEDREMIEERLKTYAHLFDDKVMKQLKRRRYTGWGRLSRKLINGIRDKQSGKTILDFLKSDGFANRNFMQLIHDDSLTFKEDIQKAQVSGQGDSLHEHIANLAGSPAIKKGILQTVKVVDELVKVMGRHKPENIVIEMARENQTTQKGQKNSRERMKRIEEGIKELGSQILKEHPVENTQLQNEKLYLYYLQNGRDMYVDQELDINRLSDYDVDAIVPQSFLKDDSIDNKVLTRSDKNRGKSDNVPSEEVVKKMKNYWRQLLNAKLITQRKFDNLTKAERGGLSELDKAGFIKRQLVETRQITKHVAQILDSRMNTKYDENDKLIREVKVITLKSKLVSDFRKDFQFYKVREINNYHHAHDAYLNAVVGTALIKKYPKLESEFVYGDYKVYDVRKMIAKSEQEIGKATAKYFFYSNIMNFFKTEITLANGEIRKRPLIETNGETGEIVWDKGRDFATVRKVLSMPQVNIVKKTEVQTGGGSSGSYGKIAALKAENAALEAKIAALKAEIAALEAGGSGGSFSKESILPKRNSDKLIARKKDWDPKKYGGFDSPTVAYSVLVVAKVEKGKSKKLKSVKELLGITIMERSSFEKNPIDFLEAKGYKEVKKDLIIKLPKYSLFELENGRKRMLASAGELQKGNELALPSKYVNFLYLASHYEKLKGSPEDNEQKQLFVEQHKHYLDEIIEQISEFSKRVILADANLDKVLSAYNKHRDKPIREQAENIIHLFTLTNLGAPAAFKYFDTTIDRKRYTSTKEVLDATLIHQSITGLYETRIDLSQLGGDDPKKKRKVEASGSGRADALDDFDLDMLGSDALDDFDLDMLGSDALDDFDLDMLGSDALDDFDLDMLINTSGGSGGGSGGSSQYLPDTDDRHRIEEKRKRTYETFKSIMKKSPFSGPTDPRPPPRRIAVPSRSSASVPKPAPQPYPFTSSLSTINYDEFPTMVFPSGQISQASALAPAPPQVLPQAPAPAPAPAMVSALAQAPAPVPVLAPGPPQAVAPPAPKPTQAGEGTLSEALLQLQFDDEDLGALLGNSTDPAVFTDLASVDNSEFQQLLNQGIPVAPHTTEPMLMEYPEAITRLVTGAQRPPDPAPAPLGAPGLPNGLLSGDEDFSSIADMDFSALLGSGSGSRDSREGMFLPKPEAGSAISDVFEGREVCQPKRIRPFHPPGSPWANRPLPASLAPTPTGPVHEPVGSLTPAPVPQPLDPAPAVTPEASHLLEDPDEETSQAVKALREMADTVIPQKEEAAICGQMDLSHPPPRGHLDELTTTLESMTEDLNLDSPLTPELNEILDTFLNDECLLHAMHISTGLSIFDTSLF</t>
+    <t>MDKKYSIGLAIGTNSVGWAVITDEYKVPSKKFKVLGNTDRHSIKKNLIGALLFDSGETAEATRLKRTARRRYTRRKNRICYLQEIFSNEMAKVDDSFFHRLEESFLVEEDKKHERHPIFGNIVDEVAYHEKYPTIYHLRKKLVDSTDKADLRLIYLALAHMIKFRGHFLIEGDLNPDNSDVDKLFIQLVQTYNQLFEENPINASGVDAKAILSARLSKSRRLENLIAQLPGEKKNGLFGNLIALSLGLTPNFKSNFDLAEDAKLQLSKDTYDDDLDNLLAQIGDQYADLFLAAKNLSDAILLSDILRVNTEITKAPLSASMIKRYDEHHQDLTLLKALVRQQLPEKYKEIFFDQSKNGYAGYIDGGASQEEFYKFIKPILEKMDGTEELLVKLNREDLLRKQRTFDNGSIPHQIHLGELHAILRRQEDFYPFLKDNREKIEKILTFRIPYYVGPLARGNSRFAWMTRKSEETITPWNFEEVVDKGASAQSFIERMTNFDKNLPNEKVLPKHSLLYEYFTVYNELTKVKYVTEGMRKPAFLSGEQKKAIVDLLFKTNRKVTVKQLKEDYFKKIECFDSVEISGVEDRFNASLGTYHDLLKIIKDKDFLDNEENEDILEDIVLTLTLFEDREMIEERLKTYAHLFDDKVMKQLKRRRYTGWGRLSRKLINGIRDKQSGKTILDFLKSDGFANRNFMQLIHDDSLTFKEDIQKAQVSGQGDSLHEHIANLAGSPAIKKGILQTVKVVDELVKVMGRHKPENIVIEMARENQTTQKGQKNSRERMKRIEEGIKELGSQILKEHPVENTQLQNEKLYLYYLQNGRDMYVDQELDINRLSDYDVDAIVPQSFLKDDSIDNKVLTRSDKNRGKSDNVPSEEVVKKMKNYWRQLLNAKLITQRKFDNLTKAERGGLSELDKAGFIKRQLVETRQITKHVAQILDSRMNTKYDENDKLIREVKVITLKSKLVSDFRKDFQFYKVREINNYHHAHDAYLNAVVGTALIKKYPKLESEFVYGDYKVYDVRKMIAKSEQEIGKATAKYFFYSNIMNFFKTEITLANGEIRKRPLIETNGETGEIVWDKGRDFATVRKVLSMPQVNIVKKTEVQTGGGSSGSYGKIAALKAENAALEAKIAALKAEIAALEAGGSGGSFSKESILPKRNSDKLIARKKDWDPKKYGGFDSPTVAYSVLVVAKVEKGKSKKLKSVKELLGITIMERSSFEKNPIDFLEAKGYKEVKKDLIIKLPKYSLFELENGRKRMLASAGELQKGNELALPSKYVNFLYLASHYEKLKGSPEDNEQKQLFVEQHKHYLDEIIEQISEFSKRVILADANLDKVLSAYNKHRDKPIREQAENIIHLFTLTNLGAPAAFKYFDTTIDRKRYTSTKEVLDATLIHQSITGLYETRIDLSQLGGDDPKKKRKVEASGSGRADALDDFDLDMLGSDALDDFDLDMLGSDALDDFDLDMLGSDALDDFDLDMLINTSGGSGGGSGGSSQYLPDTDDRHRIEEKRKRTYETFKSIMKKSPFSGPTDPRPPPRRIAVPSRSSASVPKPAPQPYPFTSSLSTINYDEFPTMVFPSGQISQASALAPAPPQVLPQAPAPAPAPAMVSALAQAPAPVPVLAPGPPQAVAPPAPKPTQAGEGTLSEALLQLQFDDEDLGALLGNSTDPAVFTDLASVDNSEFQQLLNQGIPVAPHTTEPMLMEYPEAITRLVTGAQRPPDPAPAPLGAPGLPNGLLSGDEDFSSIADMDFSALLGSGSGSRDSREGMFLPKPEAGSAISDVFEGREVCQPKRIRPFHPPGSPWANRPLPASLAPTPTGPVHEPVGSLTPAPVPQPLDPAPAVTPEASHLLEDPDEETSQAVKALREMADTVIPQKEEAAICGQMDLSHPPPRGHLDELTTTLESMTEDLNLDSPLTPELNEILDTFLNDECLLHAMHISTGLSIFDTSLF</t>
   </si>
   <si>
     <t>dCas_K1153</t>
   </si>
   <si>
-    <t>DKKYSIGLAIGTNSVGWAVITDEYKVPSKKFKVLGNTDRHSIKKNLIGALLFDSGETAEATRLKRTARRRYTRRKNRICYLQEIFSNEMAKVDDSFFHRLEESFLVEEDKKHERHPIFGNIVDEVAYHEKYPTIYHLRKKLVDSTDKADLRLIYLALAHMIKFRGHFLIEGDLNPDNSDVDKLFIQLVQTYNQLFEENPINASGVDAKAILSARLSKSRRLENLIAQLPGEKKNGLFGNLIALSLGLTPNFKSNFDLAEDAKLQLSKDTYDDDLDNLLAQIGDQYADLFLAAKNLSDAILLSDILRVNTEITKAPLSASMIKRYDEHHQDLTLLKALVRQQLPEKYKEIFFDQSKNGYAGYIDGGASQEEFYKFIKPILEKMDGTEELLVKLNREDLLRKQRTFDNGSIPHQIHLGELHAILRRQEDFYPFLKDNREKIEKILTFRIPYYVGPLARGNSRFAWMTRKSEETITPWNFEEVVDKGASAQSFIERMTNFDKNLPNEKVLPKHSLLYEYFTVYNELTKVKYVTEGMRKPAFLSGEQKKAIVDLLFKTNRKVTVKQLKEDYFKKIECFDSVEISGVEDRFNASLGTYHDLLKIIKDKDFLDNEENEDILEDIVLTLTLFEDREMIEERLKTYAHLFDDKVMKQLKRRRYTGWGRLSRKLINGIRDKQSGKTILDFLKSDGFANRNFMQLIHDDSLTFKEDIQKAQVSGQGDSLHEHIANLAGSPAIKKGILQTVKVVDELVKVMGRHKPENIVIEMARENQTTQKGQKNSRERMKRIEEGIKELGSQILKEHPVENTQLQNEKLYLYYLQNGRDMYVDQELDINRLSDYDVDAIVPQSFLKDDSIDNKVLTRSDKNRGKSDNVPSEEVVKKMKNYWRQLLNAKLITQRKFDNLTKAERGGLSELDKAGFIKRQLVETRQITKHVAQILDSRMNTKYDENDKLIREVKVITLKSKLVSDFRKDFQFYKVREINNYHHAHDAYLNAVVGTALIKKYPKLESEFVYGDYKVYDVRKMIAKSEQEIGKATAKYFFYSNIMNFFKTEITLANGEIRKRPLIETNGETGEIVWDKGRDFATVRKVLSMPQVNIVKKTEVQTGGFSKESILPKRNSDKLIARKKDWDPKKYGGFDSPTVAYSVLVVAKVEKGKSKGSSGSYGKIAALKAENAALEAKIAALKAEIAALEAGGSGGSKLKSVKELLGITIMERSSFEKNPIDFLEAKGYKEVKKDLIIKLPKYSLFELENGRKRMLASAGELQKGNELALPSKYVNFLYLASHYEKLKGSPEDNEQKQLFVEQHKHYLDEIIEQISEFSKRVILADANLDKVLSAYNKHRDKPIREQAENIIHLFTLTNLGAPAAFKYFDTTIDRKRYTSTKEVLDATLIHQSITGLYETRIDLSQLGGDDPKKKRKVEASGSGRADALDDFDLDMLGSDALDDFDLDMLGSDALDDFDLDMLGSDALDDFDLDMLINTSGGSGGGSGGSSQYLPDTDDRHRIEEKRKRTYETFKSIMKKSPFSGPTDPRPPPRRIAVPSRSSASVPKPAPQPYPFTSSLSTINYDEFPTMVFPSGQISQASALAPAPPQVLPQAPAPAPAPAMVSALAQAPAPVPVLAPGPPQAVAPPAPKPTQAGEGTLSEALLQLQFDDEDLGALLGNSTDPAVFTDLASVDNSEFQQLLNQGIPVAPHTTEPMLMEYPEAITRLVTGAQRPPDPAPAPLGAPGLPNGLLSGDEDFSSIADMDFSALLGSGSGSRDSREGMFLPKPEAGSAISDVFEGREVCQPKRIRPFHPPGSPWANRPLPASLAPTPTGPVHEPVGSLTPAPVPQPLDPAPAVTPEASHLLEDPDEETSQAVKALREMADTVIPQKEEAAICGQMDLSHPPPRGHLDELTTTLESMTEDLNLDSPLTPELNEILDTFLNDECLLHAMHISTGLSIFDTSLF</t>
+    <t>MDKKYSIGLAIGTNSVGWAVITDEYKVPSKKFKVLGNTDRHSIKKNLIGALLFDSGETAEATRLKRTARRRYTRRKNRICYLQEIFSNEMAKVDDSFFHRLEESFLVEEDKKHERHPIFGNIVDEVAYHEKYPTIYHLRKKLVDSTDKADLRLIYLALAHMIKFRGHFLIEGDLNPDNSDVDKLFIQLVQTYNQLFEENPINASGVDAKAILSARLSKSRRLENLIAQLPGEKKNGLFGNLIALSLGLTPNFKSNFDLAEDAKLQLSKDTYDDDLDNLLAQIGDQYADLFLAAKNLSDAILLSDILRVNTEITKAPLSASMIKRYDEHHQDLTLLKALVRQQLPEKYKEIFFDQSKNGYAGYIDGGASQEEFYKFIKPILEKMDGTEELLVKLNREDLLRKQRTFDNGSIPHQIHLGELHAILRRQEDFYPFLKDNREKIEKILTFRIPYYVGPLARGNSRFAWMTRKSEETITPWNFEEVVDKGASAQSFIERMTNFDKNLPNEKVLPKHSLLYEYFTVYNELTKVKYVTEGMRKPAFLSGEQKKAIVDLLFKTNRKVTVKQLKEDYFKKIECFDSVEISGVEDRFNASLGTYHDLLKIIKDKDFLDNEENEDILEDIVLTLTLFEDREMIEERLKTYAHLFDDKVMKQLKRRRYTGWGRLSRKLINGIRDKQSGKTILDFLKSDGFANRNFMQLIHDDSLTFKEDIQKAQVSGQGDSLHEHIANLAGSPAIKKGILQTVKVVDELVKVMGRHKPENIVIEMARENQTTQKGQKNSRERMKRIEEGIKELGSQILKEHPVENTQLQNEKLYLYYLQNGRDMYVDQELDINRLSDYDVDAIVPQSFLKDDSIDNKVLTRSDKNRGKSDNVPSEEVVKKMKNYWRQLLNAKLITQRKFDNLTKAERGGLSELDKAGFIKRQLVETRQITKHVAQILDSRMNTKYDENDKLIREVKVITLKSKLVSDFRKDFQFYKVREINNYHHAHDAYLNAVVGTALIKKYPKLESEFVYGDYKVYDVRKMIAKSEQEIGKATAKYFFYSNIMNFFKTEITLANGEIRKRPLIETNGETGEIVWDKGRDFATVRKVLSMPQVNIVKKTEVQTGGFSKESILPKRNSDKLIARKKDWDPKKYGGFDSPTVAYSVLVVAKVEKGKSKGSSGSYGKIAALKAENAALEAKIAALKAEIAALEAGGSGGSKLKSVKELLGITIMERSSFEKNPIDFLEAKGYKEVKKDLIIKLPKYSLFELENGRKRMLASAGELQKGNELALPSKYVNFLYLASHYEKLKGSPEDNEQKQLFVEQHKHYLDEIIEQISEFSKRVILADANLDKVLSAYNKHRDKPIREQAENIIHLFTLTNLGAPAAFKYFDTTIDRKRYTSTKEVLDATLIHQSITGLYETRIDLSQLGGDDPKKKRKVEASGSGRADALDDFDLDMLGSDALDDFDLDMLGSDALDDFDLDMLGSDALDDFDLDMLINTSGGSGGGSGGSSQYLPDTDDRHRIEEKRKRTYETFKSIMKKSPFSGPTDPRPPPRRIAVPSRSSASVPKPAPQPYPFTSSLSTINYDEFPTMVFPSGQISQASALAPAPPQVLPQAPAPAPAPAMVSALAQAPAPVPVLAPGPPQAVAPPAPKPTQAGEGTLSEALLQLQFDDEDLGALLGNSTDPAVFTDLASVDNSEFQQLLNQGIPVAPHTTEPMLMEYPEAITRLVTGAQRPPDPAPAPLGAPGLPNGLLSGDEDFSSIADMDFSALLGSGSGSRDSREGMFLPKPEAGSAISDVFEGREVCQPKRIRPFHPPGSPWANRPLPASLAPTPTGPVHEPVGSLTPAPVPQPLDPAPAVTPEASHLLEDPDEETSQAVKALREMADTVIPQKEEAAICGQMDLSHPPPRGHLDELTTTLESMTEDLNLDSPLTPELNEILDTFLNDECLLHAMHISTGLSIFDTSLF</t>
   </si>
   <si>
     <t>53,2</t>
@@ -592,7 +634,7 @@
     <t>MEDAKNIKKGPAPFYPLEDGTAGEQLHKAMKRYALVPGTIAFTDAHIEVDITYAEYFEMSVRLAEAMKRYGLNTNHRIVVCSENSLQFFMPVLGALFIGVAVAPANDIYNERELLNSMGISQPTVVFVSKKGLQKILNVQKKLPIIQKIIIMDSKTDYQGFQSMYTFVTSHLPPGFNEYDFVPESFDRDKTIALIMNSSGSTGLPKGVALPHRTACVRFSHARDPIFGNQIIPDTAILSVVPFHHGFGMFTTLGYLICGFRVVLMYRFEEELFLRSLQDYKIQSALLVPTLFSFFAKSTLIDKYDLSNLHEIASGGAPLSKEVGEAVAKRFHLPGIRQGYGLTETTSAILITPEGDDKPGAVGKVVPFFEAKVVDLDTGKTLGVNQRGELCVRGPMIMSGYVNNPEATNALIDKDGWLHSGDIAYWDEDEGSSGSEIQALEEKNAQLKQEIAALEEKNQALKYGGSGGSHFFIVDRLKSLIKYKGYQVAPAELESILLQHPNIFDAGVAGLPDDDAGELPAAVVVLEHGKTMTEKEIVDYVASQVTTAKKLRGGVVFVDEVPKGLTGKLDARKIREILIKAKKGGKIAV</t>
   </si>
   <si>
-    <t>P8</t>
+    <t>not active</t>
   </si>
   <si>
     <t>fLuc_T202_P7</t>
@@ -601,7 +643,25 @@
     <t>MGSEDAKNIKKGPAPFYPLEDGTAGEQLHKAMKRYALVPGTIAFTDAHIEVDITYAEYFEMSVRLAEAMKRYGLNTNHRIVVCSENSLQFFMPVLGALFIGVAVAPANDIYNERELLNSMGISQPTVVFVSKKGLQKILNVQKKLPIIQKIIIMDSKTDYQGFQSMYTFVTSHLPPGFNEYDFVPESFDRDKTIALIMNSSGSTGSSGSEIQALEEKNAQLKQEIAALEEKNQALKYGGSGGSGLPKGVALPHRTACVRFSHARDPIFGNQIIPDTAILSVVPFHHGFGMFTTLGYLICGFRVVLMYRFEEELFLRSLQDYKIQSALLVPTLFSFFAKSTLIDKYDLSNLHEIASGGAPLSKEVGEAVAKRFHLPGIRQGYGLTETTSAILITPEGDDKPGAVGKVVPFFEAKVVDLDTGKTLGVNQRGELCVRGPMIMSGYVNNPEATNALIDKDGWLHSGDIAYWDEDEHFFIVDRLKSLIKYKGYQVAPAELESILLQHPNIFDAGVAGLPDDDAGELPAAVVVLEHGKTMTEKEIVDYVASQVTTAKKLRGGVVFVDEVPKGLTGKLDARKIREILIKAKKGGKIAV</t>
   </si>
   <si>
-    <t>P9</t>
+    <t>fLuc_K493_N8</t>
+  </si>
+  <si>
+    <t>91,6</t>
+  </si>
+  <si>
+    <t>NT</t>
+  </si>
+  <si>
+    <t>fLuc_K493_5gs:N8</t>
+  </si>
+  <si>
+    <t>34,5</t>
+  </si>
+  <si>
+    <t>fLuc_K493_10gs:N8</t>
+  </si>
+  <si>
+    <t>3,9</t>
   </si>
 </sst>
 </file>
@@ -636,7 +696,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -703,14 +763,39 @@
         <bgColor rgb="FFACB9CA"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC27BA0"/>
+        <bgColor rgb="FFC27BA0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -724,10 +809,10 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -771,6 +856,9 @@
     <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -802,6 +890,25 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="12" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="12" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="12" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1105,33 +1212,40 @@
       <c r="I2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="3"/>
+      <c r="J2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="L2" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="5">
+        <v>29</v>
+      </c>
+      <c r="O2" s="4">
         <f t="shared" ref="O2:O60" si="1">FIND(D2&amp;E2&amp;F2,C2)-1</f>
         <v>265</v>
       </c>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
+      <c r="P2" s="5">
+        <f t="shared" ref="P2:P33" si="2">O2</f>
+        <v>265</v>
+      </c>
+      <c r="Q2" s="5"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>19</v>
@@ -1151,42 +1265,49 @@
       <c r="I3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="3"/>
+      <c r="J3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="L3" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="5">
+        <v>29</v>
+      </c>
+      <c r="O3" s="4">
         <f t="shared" si="1"/>
         <v>278</v>
       </c>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
+      <c r="P3" s="5">
+        <f t="shared" si="2"/>
+        <v>278</v>
+      </c>
+      <c r="Q3" s="5"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>22</v>
@@ -1197,42 +1318,49 @@
       <c r="I4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="3"/>
+      <c r="J4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="L4" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="5">
+        <v>29</v>
+      </c>
+      <c r="O4" s="4">
         <f t="shared" si="1"/>
         <v>375</v>
       </c>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
+      <c r="P4" s="5">
+        <f t="shared" si="2"/>
+        <v>375</v>
+      </c>
+      <c r="Q4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>22</v>
@@ -1243,36 +1371,43 @@
       <c r="I5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="3"/>
+      <c r="J5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="L5" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O5" s="5">
+        <v>29</v>
+      </c>
+      <c r="O5" s="4">
         <f t="shared" si="1"/>
         <v>255</v>
       </c>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
+      <c r="P5" s="5">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="Q5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>20</v>
@@ -1295,27 +1430,30 @@
         <v>24</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6" s="5">
+        <v>29</v>
+      </c>
+      <c r="O6" s="4">
         <f t="shared" si="1"/>
         <v>213</v>
       </c>
-      <c r="P6" s="7"/>
+      <c r="P6" s="5">
+        <f t="shared" si="2"/>
+        <v>213</v>
+      </c>
       <c r="Q6" s="7"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>19</v>
@@ -1335,33 +1473,40 @@
       <c r="I7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="6"/>
+      <c r="J7" s="6">
+        <v>54.0</v>
+      </c>
+      <c r="K7" s="6">
+        <v>3.0</v>
+      </c>
       <c r="L7" s="6" t="s">
         <v>24</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="O7" s="5">
+        <v>29</v>
+      </c>
+      <c r="O7" s="4">
         <f t="shared" si="1"/>
         <v>226</v>
       </c>
-      <c r="P7" s="7"/>
+      <c r="P7" s="5">
+        <f t="shared" si="2"/>
+        <v>226</v>
+      </c>
       <c r="Q7" s="7"/>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>19</v>
@@ -1379,35 +1524,42 @@
         <v>23</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="6"/>
+        <v>48</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="L8" s="6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="O8" s="5">
+        <v>29</v>
+      </c>
+      <c r="O8" s="4">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="P8" s="7"/>
+      <c r="P8" s="5">
+        <f t="shared" si="2"/>
+        <v>82</v>
+      </c>
       <c r="Q8" s="7"/>
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>19</v>
@@ -1427,33 +1579,40 @@
       <c r="I9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="6"/>
+      <c r="J9" s="6">
+        <v>20.0</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="L9" s="6" t="s">
         <v>24</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="O9" s="5">
+        <v>29</v>
+      </c>
+      <c r="O9" s="4">
         <f t="shared" si="1"/>
         <v>223</v>
       </c>
-      <c r="P9" s="7"/>
+      <c r="P9" s="5">
+        <f t="shared" si="2"/>
+        <v>223</v>
+      </c>
       <c r="Q9" s="7"/>
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>19</v>
@@ -1473,33 +1632,40 @@
       <c r="I10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="6"/>
+      <c r="J10" s="6">
+        <v>28.0</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="L10" s="6" t="s">
         <v>24</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="O10" s="5">
+        <v>29</v>
+      </c>
+      <c r="O10" s="4">
         <f t="shared" si="1"/>
         <v>229</v>
       </c>
-      <c r="P10" s="7"/>
+      <c r="P10" s="5">
+        <f t="shared" si="2"/>
+        <v>229</v>
+      </c>
       <c r="Q10" s="7"/>
     </row>
     <row r="11">
       <c r="A11" s="8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>19</v>
@@ -1522,32 +1688,37 @@
       <c r="J11" s="9">
         <v>82.0</v>
       </c>
-      <c r="K11" s="8"/>
+      <c r="K11" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="L11" s="8" t="s">
         <v>24</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O11" s="5">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="P11" s="10"/>
+        <v>29</v>
+      </c>
+      <c r="O11" s="4">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="P11" s="5">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
       <c r="Q11" s="10"/>
     </row>
     <row r="12">
       <c r="A12" s="8" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>19</v>
@@ -1565,37 +1736,42 @@
         <v>23</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J12" s="9">
         <v>4.0</v>
       </c>
-      <c r="K12" s="8"/>
+      <c r="K12" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="L12" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O12" s="5">
+        <v>29</v>
+      </c>
+      <c r="O12" s="4">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="P12" s="10"/>
+      <c r="P12" s="5">
+        <f t="shared" si="2"/>
+        <v>73</v>
+      </c>
       <c r="Q12" s="10"/>
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="C13" s="8" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>19</v>
@@ -1618,32 +1794,37 @@
       <c r="J13" s="9">
         <v>47.0</v>
       </c>
-      <c r="K13" s="8"/>
+      <c r="K13" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="L13" s="8" t="s">
         <v>24</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O13" s="5">
+        <v>29</v>
+      </c>
+      <c r="O13" s="4">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-      <c r="P13" s="10"/>
+      <c r="P13" s="5">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
       <c r="Q13" s="10"/>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>19</v>
@@ -1666,32 +1847,37 @@
       <c r="J14" s="9">
         <v>92.0</v>
       </c>
-      <c r="K14" s="8"/>
+      <c r="K14" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="L14" s="8" t="s">
         <v>24</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O14" s="5">
+        <v>29</v>
+      </c>
+      <c r="O14" s="4">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="P14" s="10"/>
+      <c r="P14" s="5">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
       <c r="Q14" s="10"/>
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>19</v>
@@ -1709,37 +1895,42 @@
         <v>23</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J15" s="9">
         <v>1.0</v>
       </c>
-      <c r="K15" s="8"/>
+      <c r="K15" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="L15" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O15" s="5">
+        <v>29</v>
+      </c>
+      <c r="O15" s="4">
         <f t="shared" si="1"/>
         <v>148</v>
       </c>
-      <c r="P15" s="10"/>
+      <c r="P15" s="5">
+        <f t="shared" si="2"/>
+        <v>148</v>
+      </c>
       <c r="Q15" s="10"/>
     </row>
     <row r="16">
       <c r="A16" s="8" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>19</v>
@@ -1757,37 +1948,42 @@
         <v>23</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J16" s="9">
         <v>2.0</v>
       </c>
-      <c r="K16" s="8"/>
+      <c r="K16" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="L16" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O16" s="5">
+        <v>29</v>
+      </c>
+      <c r="O16" s="4">
         <f t="shared" si="1"/>
         <v>173</v>
       </c>
-      <c r="P16" s="10"/>
+      <c r="P16" s="5">
+        <f t="shared" si="2"/>
+        <v>173</v>
+      </c>
       <c r="Q16" s="10"/>
     </row>
     <row r="17">
       <c r="A17" s="8" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>19</v>
@@ -1805,37 +2001,42 @@
         <v>23</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J17" s="9">
         <v>1.0</v>
       </c>
-      <c r="K17" s="8"/>
+      <c r="K17" s="8" t="s">
+        <v>74</v>
+      </c>
       <c r="L17" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O17" s="5">
+        <v>29</v>
+      </c>
+      <c r="O17" s="4">
         <f t="shared" si="1"/>
         <v>176</v>
       </c>
-      <c r="P17" s="10"/>
+      <c r="P17" s="5">
+        <f t="shared" si="2"/>
+        <v>176</v>
+      </c>
       <c r="Q17" s="10"/>
     </row>
     <row r="18">
       <c r="A18" s="8" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>19</v>
@@ -1853,37 +2054,42 @@
         <v>23</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J18" s="9">
         <v>1.0</v>
       </c>
-      <c r="K18" s="8"/>
+      <c r="K18" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="L18" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O18" s="5">
+        <v>29</v>
+      </c>
+      <c r="O18" s="4">
         <f t="shared" si="1"/>
         <v>185</v>
       </c>
-      <c r="P18" s="10"/>
+      <c r="P18" s="5">
+        <f t="shared" si="2"/>
+        <v>185</v>
+      </c>
       <c r="Q18" s="10"/>
     </row>
     <row r="19">
       <c r="A19" s="8" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>19</v>
@@ -1901,37 +2107,42 @@
         <v>23</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J19" s="9">
         <v>3.0</v>
       </c>
-      <c r="K19" s="8"/>
+      <c r="K19" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="L19" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N19" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O19" s="5">
+        <v>29</v>
+      </c>
+      <c r="O19" s="4">
         <f t="shared" si="1"/>
         <v>213</v>
       </c>
-      <c r="P19" s="10"/>
+      <c r="P19" s="5">
+        <f t="shared" si="2"/>
+        <v>213</v>
+      </c>
       <c r="Q19" s="10"/>
     </row>
     <row r="20">
       <c r="A20" s="8" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>19</v>
@@ -1946,38 +2157,45 @@
         <v>22</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J20" s="10"/>
-      <c r="K20" s="8"/>
+      <c r="J20" s="8">
+        <v>37.0</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>84</v>
+      </c>
       <c r="L20" s="8" t="s">
         <v>24</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="O20" s="5">
+        <v>86</v>
+      </c>
+      <c r="O20" s="4">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-      <c r="P20" s="10"/>
+      <c r="P20" s="5">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
       <c r="Q20" s="10"/>
     </row>
     <row r="21">
       <c r="A21" s="8" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>19</v>
@@ -1992,38 +2210,45 @@
         <v>22</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="10"/>
-      <c r="K21" s="8"/>
+      <c r="J21" s="8">
+        <v>60.0</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="L21" s="8" t="s">
         <v>24</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="O21" s="5">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="P21" s="10"/>
+        <v>86</v>
+      </c>
+      <c r="O21" s="4">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="P21" s="5">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
       <c r="Q21" s="10"/>
     </row>
     <row r="22">
       <c r="A22" s="8" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>19</v>
@@ -2038,50 +2263,57 @@
         <v>22</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J22" s="10"/>
-      <c r="K22" s="8"/>
+      <c r="J22" s="8">
+        <v>56.0</v>
+      </c>
+      <c r="K22" s="8">
+        <v>23.0</v>
+      </c>
       <c r="L22" s="8" t="s">
         <v>24</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="O22" s="5">
+        <v>86</v>
+      </c>
+      <c r="O22" s="4">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="P22" s="10"/>
+      <c r="P22" s="5">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
       <c r="Q22" s="10"/>
     </row>
     <row r="23">
       <c r="A23" s="11" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>19</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="F23" s="11" t="s">
         <v>19</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>23</v>
@@ -2097,42 +2329,45 @@
         <v>24</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="N23" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="O23" s="5">
+        <v>98</v>
+      </c>
+      <c r="O23" s="4">
         <f t="shared" si="1"/>
         <v>524</v>
       </c>
-      <c r="P23" s="13"/>
+      <c r="P23" s="5">
+        <f t="shared" si="2"/>
+        <v>524</v>
+      </c>
       <c r="Q23" s="13"/>
     </row>
     <row r="24">
       <c r="A24" s="11" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>19</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="F24" s="11" t="s">
         <v>19</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="I24" s="11" t="s">
         <v>24</v>
@@ -2145,42 +2380,45 @@
         <v>24</v>
       </c>
       <c r="M24" s="11" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="N24" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="O24" s="5">
+        <v>98</v>
+      </c>
+      <c r="O24" s="4">
         <f t="shared" si="1"/>
         <v>593</v>
       </c>
-      <c r="P24" s="13"/>
+      <c r="P24" s="5">
+        <f t="shared" si="2"/>
+        <v>593</v>
+      </c>
       <c r="Q24" s="13"/>
     </row>
     <row r="25">
       <c r="A25" s="11" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>19</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>19</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="I25" s="11" t="s">
         <v>24</v>
@@ -2191,135 +2429,144 @@
         <v>24</v>
       </c>
       <c r="M25" s="11" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="N25" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="O25" s="5">
+        <v>105</v>
+      </c>
+      <c r="O25" s="4">
         <f t="shared" si="1"/>
         <v>595</v>
       </c>
-      <c r="P25" s="13"/>
+      <c r="P25" s="5">
+        <f t="shared" si="2"/>
+        <v>595</v>
+      </c>
       <c r="Q25" s="13"/>
     </row>
     <row r="26">
       <c r="A26" s="14" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H26" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="K26" s="14"/>
       <c r="L26" s="14" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M26" s="14" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N26" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="O26" s="5">
+        <v>86</v>
+      </c>
+      <c r="O26" s="4">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="P26" s="16"/>
+      <c r="P26" s="5">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
       <c r="Q26" s="16"/>
     </row>
     <row r="27">
       <c r="A27" s="14" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H27" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="K27" s="14"/>
       <c r="L27" s="14" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M27" s="14" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N27" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="O27" s="5">
+        <v>86</v>
+      </c>
+      <c r="O27" s="4">
         <f t="shared" si="1"/>
         <v>147</v>
       </c>
-      <c r="P27" s="16"/>
+      <c r="P27" s="5">
+        <f t="shared" si="2"/>
+        <v>147</v>
+      </c>
       <c r="Q27" s="16"/>
     </row>
     <row r="28">
       <c r="A28" s="14" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H28" s="14" t="s">
         <v>23</v>
@@ -2328,94 +2575,100 @@
         <v>24</v>
       </c>
       <c r="J28" s="15" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="K28" s="14"/>
       <c r="L28" s="14" t="s">
         <v>24</v>
       </c>
       <c r="M28" s="14" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N28" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="O28" s="5">
+        <v>86</v>
+      </c>
+      <c r="O28" s="4">
         <f t="shared" si="1"/>
         <v>535</v>
       </c>
-      <c r="P28" s="16"/>
+      <c r="P28" s="5">
+        <f t="shared" si="2"/>
+        <v>535</v>
+      </c>
       <c r="Q28" s="16"/>
     </row>
     <row r="29">
       <c r="A29" s="14" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H29" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J29" s="15" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="K29" s="14"/>
       <c r="L29" s="14" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M29" s="14" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N29" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="O29" s="5">
-        <f t="shared" si="1"/>
-        <v>1103</v>
-      </c>
-      <c r="P29" s="16"/>
+        <v>86</v>
+      </c>
+      <c r="O29" s="4">
+        <f t="shared" si="1"/>
+        <v>1104</v>
+      </c>
+      <c r="P29" s="5">
+        <f t="shared" si="2"/>
+        <v>1104</v>
+      </c>
       <c r="Q29" s="16"/>
     </row>
     <row r="30">
       <c r="A30" s="14" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H30" s="14" t="s">
         <v>23</v>
@@ -2424,34 +2677,37 @@
         <v>24</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="K30" s="14"/>
       <c r="L30" s="14" t="s">
         <v>24</v>
       </c>
       <c r="M30" s="14" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N30" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="O30" s="5">
-        <f t="shared" si="1"/>
-        <v>1154</v>
-      </c>
-      <c r="P30" s="16"/>
+        <v>86</v>
+      </c>
+      <c r="O30" s="4">
+        <f t="shared" si="1"/>
+        <v>1155</v>
+      </c>
+      <c r="P30" s="5">
+        <f t="shared" si="2"/>
+        <v>1155</v>
+      </c>
       <c r="Q30" s="16"/>
     </row>
     <row r="31">
       <c r="A31" s="14" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>19</v>
@@ -2466,7 +2722,7 @@
         <v>22</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="I31" s="14" t="s">
         <v>24</v>
@@ -2477,27 +2733,30 @@
         <v>24</v>
       </c>
       <c r="M31" s="14" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N31" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="O31" s="5">
+        <v>86</v>
+      </c>
+      <c r="O31" s="4">
         <f t="shared" si="1"/>
         <v>605</v>
       </c>
-      <c r="P31" s="16"/>
+      <c r="P31" s="5">
+        <f t="shared" si="2"/>
+        <v>605</v>
+      </c>
       <c r="Q31" s="16"/>
     </row>
     <row r="32">
       <c r="A32" s="14" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>19</v>
@@ -2512,7 +2771,7 @@
         <v>22</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="I32" s="14" t="s">
         <v>24</v>
@@ -2523,135 +2782,144 @@
         <v>24</v>
       </c>
       <c r="M32" s="14" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N32" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="O32" s="5">
+        <v>86</v>
+      </c>
+      <c r="O32" s="4">
         <f t="shared" si="1"/>
         <v>605</v>
       </c>
-      <c r="P32" s="16"/>
+      <c r="P32" s="5">
+        <f t="shared" si="2"/>
+        <v>605</v>
+      </c>
       <c r="Q32" s="16"/>
     </row>
     <row r="33">
       <c r="A33" s="17" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>19</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H33" s="17" t="s">
         <v>23</v>
       </c>
       <c r="I33" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J33" s="18" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="K33" s="17"/>
       <c r="L33" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M33" s="17" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N33" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="O33" s="5">
+        <v>86</v>
+      </c>
+      <c r="O33" s="4">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="P33" s="19"/>
+      <c r="P33" s="5">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
       <c r="Q33" s="19"/>
     </row>
     <row r="34">
       <c r="A34" s="17" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>19</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H34" s="17" t="s">
         <v>23</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J34" s="18" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="K34" s="17"/>
       <c r="L34" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M34" s="17" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N34" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="O34" s="5">
+        <v>86</v>
+      </c>
+      <c r="O34" s="4">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="P34" s="19"/>
+      <c r="P34" s="20">
+        <f t="shared" ref="P34:P44" si="3">O34+1</f>
+        <v>27</v>
+      </c>
       <c r="Q34" s="19"/>
     </row>
     <row r="35">
       <c r="A35" s="17" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>19</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H35" s="17" t="s">
         <v>23</v>
@@ -2660,94 +2928,100 @@
         <v>24</v>
       </c>
       <c r="J35" s="18" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="K35" s="17"/>
       <c r="L35" s="17" t="s">
         <v>24</v>
       </c>
       <c r="M35" s="17" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N35" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="O35" s="5">
+        <v>86</v>
+      </c>
+      <c r="O35" s="4">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="P35" s="19"/>
+      <c r="P35" s="20">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
       <c r="Q35" s="19"/>
     </row>
     <row r="36">
       <c r="A36" s="17" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="D36" s="17" t="s">
         <v>19</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H36" s="17" t="s">
         <v>23</v>
       </c>
       <c r="I36" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J36" s="18" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="K36" s="17"/>
       <c r="L36" s="17" t="s">
         <v>24</v>
       </c>
       <c r="M36" s="17" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N36" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="O36" s="5">
+        <v>86</v>
+      </c>
+      <c r="O36" s="4">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="P36" s="19"/>
+      <c r="P36" s="20">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
       <c r="Q36" s="19"/>
     </row>
     <row r="37">
       <c r="A37" s="17" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="D37" s="17" t="s">
         <v>19</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H37" s="17" t="s">
         <v>23</v>
@@ -2756,94 +3030,100 @@
         <v>24</v>
       </c>
       <c r="J37" s="18" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="K37" s="17"/>
       <c r="L37" s="17" t="s">
         <v>24</v>
       </c>
       <c r="M37" s="17" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N37" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="O37" s="5">
+        <v>86</v>
+      </c>
+      <c r="O37" s="4">
         <f t="shared" si="1"/>
         <v>225</v>
       </c>
-      <c r="P37" s="19"/>
+      <c r="P37" s="20">
+        <f t="shared" si="3"/>
+        <v>226</v>
+      </c>
       <c r="Q37" s="19"/>
     </row>
     <row r="38">
       <c r="A38" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B38" s="17" t="s">
-        <v>114</v>
-      </c>
       <c r="C38" s="17" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="D38" s="17" t="s">
         <v>19</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H38" s="17" t="s">
         <v>23</v>
       </c>
       <c r="I38" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J38" s="18" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="K38" s="17"/>
       <c r="L38" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M38" s="17" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N38" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="O38" s="5">
+        <v>86</v>
+      </c>
+      <c r="O38" s="4">
         <f t="shared" si="1"/>
         <v>220</v>
       </c>
-      <c r="P38" s="19"/>
+      <c r="P38" s="20">
+        <f t="shared" si="3"/>
+        <v>221</v>
+      </c>
       <c r="Q38" s="19"/>
     </row>
     <row r="39">
       <c r="A39" s="17" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="D39" s="17" t="s">
         <v>19</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H39" s="17" t="s">
         <v>23</v>
@@ -2852,882 +3132,939 @@
         <v>24</v>
       </c>
       <c r="J39" s="18" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="K39" s="17"/>
       <c r="L39" s="17" t="s">
         <v>24</v>
       </c>
       <c r="M39" s="17" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N39" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="O39" s="5">
+        <v>86</v>
+      </c>
+      <c r="O39" s="4">
         <f t="shared" si="1"/>
         <v>230</v>
       </c>
-      <c r="P39" s="19"/>
+      <c r="P39" s="20">
+        <f t="shared" si="3"/>
+        <v>231</v>
+      </c>
       <c r="Q39" s="19"/>
     </row>
     <row r="40">
       <c r="A40" s="17" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="D40" s="17" t="s">
         <v>19</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H40" s="17" t="s">
         <v>23</v>
       </c>
       <c r="I40" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J40" s="18" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="K40" s="17"/>
       <c r="L40" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M40" s="17" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N40" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="O40" s="5">
+        <v>86</v>
+      </c>
+      <c r="O40" s="4">
         <f t="shared" si="1"/>
         <v>499</v>
       </c>
-      <c r="P40" s="19"/>
+      <c r="P40" s="20">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
       <c r="Q40" s="19"/>
     </row>
     <row r="41">
       <c r="A41" s="17" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="D41" s="17" t="s">
         <v>19</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H41" s="17" t="s">
         <v>23</v>
       </c>
       <c r="I41" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J41" s="18" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="K41" s="17"/>
       <c r="L41" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M41" s="17" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N41" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="O41" s="5">
+        <v>86</v>
+      </c>
+      <c r="O41" s="4">
         <f t="shared" si="1"/>
         <v>505</v>
       </c>
-      <c r="P41" s="19"/>
+      <c r="P41" s="20">
+        <f t="shared" si="3"/>
+        <v>506</v>
+      </c>
       <c r="Q41" s="19"/>
     </row>
     <row r="42">
       <c r="A42" s="17" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="D42" s="17" t="s">
         <v>19</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H42" s="17" t="s">
         <v>23</v>
       </c>
       <c r="I42" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J42" s="18" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="K42" s="17"/>
       <c r="L42" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M42" s="17" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N42" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="O42" s="5">
+        <v>86</v>
+      </c>
+      <c r="O42" s="4">
         <f t="shared" si="1"/>
         <v>602</v>
       </c>
-      <c r="P42" s="19"/>
+      <c r="P42" s="20">
+        <f t="shared" si="3"/>
+        <v>603</v>
+      </c>
       <c r="Q42" s="19"/>
     </row>
     <row r="43">
       <c r="A43" s="17" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="D43" s="17" t="s">
         <v>19</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H43" s="17" t="s">
         <v>23</v>
       </c>
       <c r="I43" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J43" s="18" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="K43" s="17"/>
       <c r="L43" s="17" t="s">
         <v>24</v>
       </c>
       <c r="M43" s="17" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="N43" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="O43" s="5">
+        <v>86</v>
+      </c>
+      <c r="O43" s="4">
         <f t="shared" si="1"/>
         <v>791</v>
       </c>
-      <c r="P43" s="19"/>
+      <c r="P43" s="20">
+        <f t="shared" si="3"/>
+        <v>792</v>
+      </c>
       <c r="Q43" s="19"/>
     </row>
     <row r="44">
       <c r="A44" s="17" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="D44" s="17" t="s">
         <v>19</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H44" s="17" t="s">
         <v>23</v>
       </c>
       <c r="I44" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J44" s="18" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="K44" s="17"/>
       <c r="L44" s="17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M44" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="N44" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="O44" s="4">
+        <f t="shared" si="1"/>
+        <v>992</v>
+      </c>
+      <c r="P44" s="5">
+        <f t="shared" si="3"/>
+        <v>993</v>
+      </c>
+      <c r="Q44" s="19"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="F45" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G45" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H45" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I45" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="J45" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="M45" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="N45" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="O45" s="4">
+        <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="N44" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="O44" s="5">
-        <f t="shared" si="1"/>
-        <v>992</v>
-      </c>
-      <c r="P44" s="19"/>
-      <c r="Q44" s="19"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="D45" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E45" s="20" t="s">
+      <c r="P45" s="5">
+        <f t="shared" ref="P45:P55" si="4">O45</f>
+        <v>72</v>
+      </c>
+      <c r="Q45" s="23"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="F46" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H46" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I46" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J46" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="M46" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="N46" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="O46" s="4">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="P46" s="5">
+        <f t="shared" si="4"/>
+        <v>86</v>
+      </c>
+      <c r="Q46" s="23"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="F47" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G47" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H47" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I47" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J47" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="K47" s="21"/>
+      <c r="L47" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M47" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="N47" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="O47" s="4">
+        <f t="shared" si="1"/>
+        <v>176</v>
+      </c>
+      <c r="P47" s="5">
+        <f t="shared" si="4"/>
+        <v>176</v>
+      </c>
+      <c r="Q47" s="23"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="F48" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G48" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H48" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I48" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J48" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="K48" s="21"/>
+      <c r="L48" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M48" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="N48" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="O48" s="4">
+        <f t="shared" si="1"/>
+        <v>215</v>
+      </c>
+      <c r="P48" s="5">
+        <f t="shared" si="4"/>
+        <v>215</v>
+      </c>
+      <c r="Q48" s="23"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="F49" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G49" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H49" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I49" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J49" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="K49" s="21"/>
+      <c r="L49" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M49" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="N49" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="O49" s="4">
+        <f t="shared" si="1"/>
+        <v>230</v>
+      </c>
+      <c r="P49" s="5">
+        <f t="shared" si="4"/>
+        <v>230</v>
+      </c>
+      <c r="Q49" s="23"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="B50" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="C50" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="D50" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E50" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F50" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="G50" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="H50" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I50" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="J50" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="K50" s="24"/>
+      <c r="L50" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="M50" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="N50" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="O50" s="4">
+        <f t="shared" si="1"/>
+        <v>212</v>
+      </c>
+      <c r="P50" s="5">
+        <f t="shared" si="4"/>
+        <v>212</v>
+      </c>
+      <c r="Q50" s="26"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="B51" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="C51" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="D51" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E51" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F51" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="G51" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="H51" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I51" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="J51" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="K51" s="24"/>
+      <c r="L51" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="M51" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="N51" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="O51" s="4">
+        <f t="shared" si="1"/>
+        <v>221</v>
+      </c>
+      <c r="P51" s="5">
+        <f t="shared" si="4"/>
+        <v>221</v>
+      </c>
+      <c r="Q51" s="26"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="B52" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="C52" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="D52" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E52" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F52" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="G52" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="H52" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I52" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="J52" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="K52" s="24"/>
+      <c r="L52" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="M52" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="N52" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="O52" s="4">
+        <f t="shared" si="1"/>
+        <v>232</v>
+      </c>
+      <c r="P52" s="5">
+        <f t="shared" si="4"/>
+        <v>232</v>
+      </c>
+      <c r="Q52" s="26"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="B53" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="D53" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E53" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F53" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="G53" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="H53" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I53" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="J53" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="K53" s="24"/>
+      <c r="L53" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="M53" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="N53" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="O53" s="4">
+        <f t="shared" si="1"/>
+        <v>281</v>
+      </c>
+      <c r="P53" s="5">
+        <f t="shared" si="4"/>
+        <v>281</v>
+      </c>
+      <c r="Q53" s="26"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="B54" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="C54" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="D54" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F54" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G54" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H54" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="I54" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="J54" s="28"/>
+      <c r="K54" s="28"/>
+      <c r="L54" s="28"/>
+      <c r="M54" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="N54" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="O54" s="4">
+        <f t="shared" si="1"/>
         <v>151</v>
       </c>
-      <c r="F45" s="20" t="s">
+      <c r="P54" s="5">
+        <f t="shared" si="4"/>
+        <v>151</v>
+      </c>
+      <c r="Q54" s="28"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="B55" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="C55" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="D55" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="G45" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="H45" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I45" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="J45" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="K45" s="20"/>
-      <c r="L45" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="M45" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="N45" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="O45" s="5">
-        <f t="shared" si="1"/>
-        <v>72</v>
-      </c>
-      <c r="P45" s="22"/>
-      <c r="Q45" s="22"/>
-    </row>
-    <row r="46">
-      <c r="A46" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E46" s="20" t="s">
+      <c r="G55" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H55" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="I55" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="J55" s="28"/>
+      <c r="K55" s="28"/>
+      <c r="L55" s="28"/>
+      <c r="M55" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="N55" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="O55" s="4">
+        <f t="shared" si="1"/>
         <v>151</v>
       </c>
-      <c r="F46" s="20" t="s">
+      <c r="P55" s="5">
+        <f t="shared" si="4"/>
+        <v>151</v>
+      </c>
+      <c r="Q55" s="28"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="B56" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="C56" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="D56" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F56" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="G46" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="H46" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I46" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J46" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="K46" s="20"/>
-      <c r="L46" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="M46" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="N46" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="O46" s="5">
-        <f t="shared" si="1"/>
+      <c r="G56" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H56" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="I56" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="J56" s="28"/>
+      <c r="K56" s="28"/>
+      <c r="L56" s="28"/>
+      <c r="M56" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="N56" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="O56" s="4">
+        <f t="shared" si="1"/>
+        <v>214</v>
+      </c>
+      <c r="P56" s="20">
+        <f>O56+2</f>
+        <v>216</v>
+      </c>
+      <c r="Q56" s="28"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="B57" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="C57" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="D57" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F57" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G57" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H57" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="I57" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="J57" s="28"/>
+      <c r="K57" s="28"/>
+      <c r="L57" s="28"/>
+      <c r="M57" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="N57" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="P46" s="22"/>
-      <c r="Q46" s="22"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="B47" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="D47" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E47" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="F47" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="G47" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="H47" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I47" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J47" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="K47" s="20"/>
-      <c r="L47" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="M47" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="N47" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="O47" s="5">
-        <f t="shared" si="1"/>
-        <v>176</v>
-      </c>
-      <c r="P47" s="22"/>
-      <c r="Q47" s="22"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="B48" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E48" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="F48" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="G48" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="H48" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I48" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J48" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="K48" s="20"/>
-      <c r="L48" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="M48" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="N48" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="O48" s="5">
-        <f t="shared" si="1"/>
-        <v>215</v>
-      </c>
-      <c r="P48" s="22"/>
-      <c r="Q48" s="22"/>
-    </row>
-    <row r="49">
-      <c r="A49" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="B49" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="C49" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="D49" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E49" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="F49" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="G49" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="H49" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I49" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J49" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="K49" s="20"/>
-      <c r="L49" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="M49" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="N49" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="O49" s="5">
-        <f t="shared" si="1"/>
-        <v>230</v>
-      </c>
-      <c r="P49" s="22"/>
-      <c r="Q49" s="22"/>
-    </row>
-    <row r="50">
-      <c r="A50" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="B50" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="C50" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="D50" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E50" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F50" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="G50" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="H50" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="I50" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="J50" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="K50" s="23"/>
-      <c r="L50" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="M50" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="N50" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="O50" s="5">
-        <f t="shared" si="1"/>
-        <v>212</v>
-      </c>
-      <c r="P50" s="25"/>
-      <c r="Q50" s="25"/>
-    </row>
-    <row r="51">
-      <c r="A51" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="B51" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="C51" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="D51" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E51" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F51" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="G51" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="H51" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="I51" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="J51" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="K51" s="23"/>
-      <c r="L51" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="M51" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="N51" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="O51" s="5">
-        <f t="shared" si="1"/>
-        <v>221</v>
-      </c>
-      <c r="P51" s="25"/>
-      <c r="Q51" s="25"/>
-    </row>
-    <row r="52">
-      <c r="A52" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="B52" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="C52" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="D52" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E52" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F52" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="G52" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="H52" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="I52" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="J52" s="24" t="s">
-        <v>174</v>
-      </c>
-      <c r="K52" s="23"/>
-      <c r="L52" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="M52" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="N52" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="O52" s="5">
-        <f t="shared" si="1"/>
-        <v>232</v>
-      </c>
-      <c r="P52" s="25"/>
-      <c r="Q52" s="25"/>
-    </row>
-    <row r="53">
-      <c r="A53" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="B53" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="C53" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="D53" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E53" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F53" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="G53" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="H53" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="I53" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="J53" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="K53" s="23"/>
-      <c r="L53" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="M53" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="N53" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="O53" s="5">
-        <f t="shared" si="1"/>
-        <v>281</v>
-      </c>
-      <c r="P53" s="25"/>
-      <c r="Q53" s="25"/>
-    </row>
-    <row r="54">
-      <c r="A54" s="26" t="s">
-        <v>178</v>
-      </c>
-      <c r="B54" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="C54" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="D54" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="E54" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F54" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="G54" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="H54" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="I54" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="J54" s="27"/>
-      <c r="K54" s="27"/>
-      <c r="L54" s="27"/>
-      <c r="M54" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="N54" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="O54" s="5">
-        <f t="shared" si="1"/>
-        <v>151</v>
-      </c>
-      <c r="P54" s="27"/>
-      <c r="Q54" s="27"/>
-    </row>
-    <row r="55">
-      <c r="A55" s="26" t="s">
-        <v>181</v>
-      </c>
-      <c r="B55" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="C55" s="26" t="s">
-        <v>183</v>
-      </c>
-      <c r="D55" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="E55" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F55" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="G55" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="H55" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="I55" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="J55" s="27"/>
-      <c r="K55" s="27"/>
-      <c r="L55" s="27"/>
-      <c r="M55" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="N55" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="O55" s="5">
-        <f t="shared" si="1"/>
-        <v>151</v>
-      </c>
-      <c r="P55" s="27"/>
-      <c r="Q55" s="27"/>
-    </row>
-    <row r="56">
-      <c r="A56" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="B56" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="C56" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="D56" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="E56" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F56" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="G56" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="H56" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="I56" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="J56" s="27"/>
-      <c r="K56" s="27"/>
-      <c r="L56" s="27"/>
-      <c r="M56" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="N56" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="O56" s="5">
+      <c r="O57" s="4">
         <f t="shared" si="1"/>
         <v>214</v>
       </c>
-      <c r="P56" s="27"/>
-      <c r="Q56" s="27"/>
-    </row>
-    <row r="57">
-      <c r="A57" s="26" t="s">
-        <v>186</v>
-      </c>
-      <c r="B57" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="C57" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="D57" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="E57" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F57" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="G57" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="H57" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="I57" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="J57" s="27"/>
-      <c r="K57" s="27"/>
-      <c r="L57" s="27"/>
-      <c r="M57" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="N57" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="O57" s="5">
-        <f t="shared" si="1"/>
+      <c r="P57" s="5">
+        <f t="shared" ref="P57:P58" si="5">O57</f>
         <v>214</v>
       </c>
-      <c r="P57" s="27"/>
-      <c r="Q57" s="27"/>
+      <c r="Q57" s="28"/>
     </row>
     <row r="58">
-      <c r="A58" s="28" t="s">
-        <v>188</v>
+      <c r="A58" s="29" t="s">
+        <v>202</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="C58" s="28" t="s">
-        <v>190</v>
+        <v>203</v>
+      </c>
+      <c r="C58" s="29" t="s">
+        <v>204</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>19</v>
@@ -3747,27 +4084,30 @@
       <c r="I58" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J58" s="10"/>
+      <c r="J58" s="8"/>
       <c r="K58" s="10"/>
-      <c r="L58" s="10"/>
+      <c r="L58" s="8"/>
       <c r="M58" s="10"/>
       <c r="N58" s="10"/>
-      <c r="O58" s="5">
+      <c r="O58" s="4">
         <f t="shared" si="1"/>
         <v>494</v>
       </c>
-      <c r="P58" s="10"/>
+      <c r="P58" s="5">
+        <f t="shared" si="5"/>
+        <v>494</v>
+      </c>
       <c r="Q58" s="10"/>
     </row>
     <row r="59">
-      <c r="A59" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="B59" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="C59" s="29" t="s">
-        <v>192</v>
+      <c r="A59" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="B59" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="C59" s="30" t="s">
+        <v>206</v>
       </c>
       <c r="D59" s="8" t="s">
         <v>19</v>
@@ -3779,35 +4119,42 @@
         <v>21</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>193</v>
+        <v>22</v>
       </c>
       <c r="H59" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I59" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="J59" s="30"/>
-      <c r="K59" s="30"/>
-      <c r="L59" s="30"/>
-      <c r="M59" s="30"/>
-      <c r="N59" s="30"/>
-      <c r="O59" s="5">
+      <c r="I59" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="J59" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="K59" s="31"/>
+      <c r="L59" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M59" s="31"/>
+      <c r="N59" s="31"/>
+      <c r="O59" s="4">
         <f t="shared" si="1"/>
         <v>430</v>
       </c>
-      <c r="P59" s="30"/>
-      <c r="Q59" s="30"/>
+      <c r="P59" s="20">
+        <f t="shared" ref="P59:P60" si="6">O59+1</f>
+        <v>431</v>
+      </c>
+      <c r="Q59" s="31"/>
     </row>
     <row r="60">
-      <c r="A60" s="29" t="s">
-        <v>194</v>
-      </c>
-      <c r="B60" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="C60" s="29" t="s">
-        <v>195</v>
+      <c r="A60" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="B60" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="C60" s="30" t="s">
+        <v>209</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>19</v>
@@ -3819,25 +4166,192 @@
         <v>21</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>196</v>
+        <v>22</v>
       </c>
       <c r="H60" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I60" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="J60" s="30"/>
-      <c r="K60" s="30"/>
-      <c r="L60" s="30"/>
-      <c r="M60" s="30"/>
-      <c r="N60" s="30"/>
-      <c r="O60" s="5">
+      <c r="I60" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="J60" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="K60" s="31"/>
+      <c r="L60" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M60" s="31"/>
+      <c r="N60" s="31"/>
+      <c r="O60" s="4">
         <f t="shared" si="1"/>
         <v>204</v>
       </c>
-      <c r="P60" s="30"/>
-      <c r="Q60" s="30"/>
+      <c r="P60" s="20">
+        <f t="shared" si="6"/>
+        <v>205</v>
+      </c>
+      <c r="Q60" s="31"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="B61" s="33"/>
+      <c r="C61" s="33"/>
+      <c r="D61" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E61" s="33"/>
+      <c r="F61" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="G61" s="33"/>
+      <c r="H61" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="I61" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="J61" s="33"/>
+      <c r="K61" s="35" t="s">
+        <v>211</v>
+      </c>
+      <c r="L61" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="M61" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="N61" s="33"/>
+      <c r="O61" s="33"/>
+      <c r="P61" s="34">
+        <v>-1.0</v>
+      </c>
+      <c r="Q61" s="33"/>
+      <c r="R61" s="33"/>
+      <c r="S61" s="33"/>
+      <c r="T61" s="33"/>
+      <c r="U61" s="33"/>
+      <c r="V61" s="33"/>
+      <c r="W61" s="33"/>
+      <c r="X61" s="33"/>
+      <c r="Y61" s="33"/>
+      <c r="Z61" s="33"/>
+      <c r="AA61" s="33"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="B62" s="33"/>
+      <c r="C62" s="33"/>
+      <c r="D62" s="33"/>
+      <c r="E62" s="33"/>
+      <c r="F62" s="33"/>
+      <c r="G62" s="33"/>
+      <c r="H62" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="I62" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="J62" s="33"/>
+      <c r="K62" s="35" t="s">
+        <v>214</v>
+      </c>
+      <c r="L62" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="M62" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="N62" s="33"/>
+      <c r="O62" s="33"/>
+      <c r="P62" s="34">
+        <v>-1.0</v>
+      </c>
+      <c r="Q62" s="33"/>
+      <c r="R62" s="33"/>
+      <c r="S62" s="33"/>
+      <c r="T62" s="33"/>
+      <c r="U62" s="33"/>
+      <c r="V62" s="33"/>
+      <c r="W62" s="33"/>
+      <c r="X62" s="33"/>
+      <c r="Y62" s="33"/>
+      <c r="Z62" s="33"/>
+      <c r="AA62" s="33"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="B63" s="33"/>
+      <c r="C63" s="33"/>
+      <c r="D63" s="33"/>
+      <c r="E63" s="33"/>
+      <c r="F63" s="33"/>
+      <c r="G63" s="33"/>
+      <c r="H63" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="I63" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="J63" s="33"/>
+      <c r="K63" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="L63" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="M63" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="N63" s="33"/>
+      <c r="O63" s="33"/>
+      <c r="P63" s="34">
+        <v>-1.0</v>
+      </c>
+      <c r="Q63" s="33"/>
+      <c r="R63" s="33"/>
+      <c r="S63" s="33"/>
+      <c r="T63" s="33"/>
+      <c r="U63" s="33"/>
+      <c r="V63" s="33"/>
+      <c r="W63" s="33"/>
+      <c r="X63" s="33"/>
+      <c r="Y63" s="33"/>
+      <c r="Z63" s="33"/>
+      <c r="AA63" s="33"/>
+    </row>
+    <row r="65">
+      <c r="G65" s="36"/>
+    </row>
+    <row r="66">
+      <c r="G66" s="37"/>
+    </row>
+    <row r="67">
+      <c r="G67" s="38"/>
+    </row>
+    <row r="68">
+      <c r="G68" s="37"/>
+    </row>
+    <row r="69">
+      <c r="G69" s="36"/>
+    </row>
+    <row r="70">
+      <c r="G70" s="37"/>
+    </row>
+    <row r="71">
+      <c r="G71" s="38"/>
+    </row>
+    <row r="72">
+      <c r="G72" s="37"/>
+    </row>
+    <row r="73">
+      <c r="G73" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>